<commit_message>
Eviscerator skills rework. Contributed by Thonygez.
</commit_message>
<xml_diff>
--- a/trunk/dist/game/data/stats/skills/TODO.xlsx
+++ b/trunk/dist/game/data/stats/skills/TODO.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1398" uniqueCount="657">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1405" uniqueCount="657">
   <si>
     <t>Skill Name</t>
   </si>
@@ -2468,7 +2468,7 @@
       </c>
       <c r="G2" s="2">
         <f>COUNTIF(C2:C679,"yes")</f>
-        <v>485</v>
+        <v>492</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -2487,7 +2487,7 @@
       </c>
       <c r="G3">
         <f>678-G2</f>
-        <v>193</v>
+        <v>186</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -2506,7 +2506,7 @@
       </c>
       <c r="G4" s="4">
         <f>100-(G3*100)/678</f>
-        <v>71.533923303834811</v>
+        <v>72.56637168141593</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -10362,7 +10362,9 @@
       <c r="B651" s="7">
         <v>30505</v>
       </c>
-      <c r="C651" s="13"/>
+      <c r="C651" s="15" t="s">
+        <v>549</v>
+      </c>
       <c r="D651" s="13"/>
     </row>
     <row r="652" spans="1:4">
@@ -10372,7 +10374,9 @@
       <c r="B652" s="7">
         <v>30506</v>
       </c>
-      <c r="C652" s="13"/>
+      <c r="C652" s="15" t="s">
+        <v>549</v>
+      </c>
       <c r="D652" s="13"/>
     </row>
     <row r="653" spans="1:4">
@@ -10382,7 +10386,9 @@
       <c r="B653" s="7">
         <v>30507</v>
       </c>
-      <c r="C653" s="13"/>
+      <c r="C653" s="15" t="s">
+        <v>549</v>
+      </c>
       <c r="D653" s="13"/>
     </row>
     <row r="654" spans="1:4">
@@ -10392,7 +10398,9 @@
       <c r="B654" s="7">
         <v>30508</v>
       </c>
-      <c r="C654" s="13"/>
+      <c r="C654" s="15" t="s">
+        <v>549</v>
+      </c>
       <c r="D654" s="13"/>
     </row>
     <row r="655" spans="1:4">
@@ -10492,7 +10500,9 @@
       <c r="B663" s="7">
         <v>30518</v>
       </c>
-      <c r="C663" s="13"/>
+      <c r="C663" s="15" t="s">
+        <v>549</v>
+      </c>
       <c r="D663" s="14" t="s">
         <v>565</v>
       </c>
@@ -10626,7 +10636,9 @@
       <c r="B675" s="7">
         <v>30546</v>
       </c>
-      <c r="C675" s="13"/>
+      <c r="C675" s="15" t="s">
+        <v>549</v>
+      </c>
       <c r="D675" s="13"/>
     </row>
     <row r="676" spans="1:4">
@@ -10636,7 +10648,9 @@
       <c r="B676" s="7">
         <v>30547</v>
       </c>
-      <c r="C676" s="13"/>
+      <c r="C676" s="15" t="s">
+        <v>549</v>
+      </c>
       <c r="D676" s="13"/>
     </row>
     <row r="677" spans="1:4">

</xml_diff>

<commit_message>
Flying Body Reinforcement skill (1954).
</commit_message>
<xml_diff>
--- a/trunk/dist/game/data/stats/skills/TODO.xlsx
+++ b/trunk/dist/game/data/stats/skills/TODO.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1403" uniqueCount="656">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1404" uniqueCount="656">
   <si>
     <t>Skill Name</t>
   </si>
@@ -2465,7 +2465,7 @@
       </c>
       <c r="G2" s="2">
         <f>COUNTIF(C2:C679,"yes")</f>
-        <v>495</v>
+        <v>496</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -2484,7 +2484,7 @@
       </c>
       <c r="G3">
         <f>678-G2</f>
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -2503,7 +2503,7 @@
       </c>
       <c r="G4" s="4">
         <f>100-(G3*100)/678</f>
-        <v>73.008849557522126</v>
+        <v>73.156342182890853</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -3089,7 +3089,9 @@
       <c r="B53" s="7">
         <v>1954</v>
       </c>
-      <c r="C53" s="14"/>
+      <c r="C53" s="8" t="s">
+        <v>549</v>
+      </c>
       <c r="D53" s="12"/>
     </row>
     <row r="54" spans="1:4">

</xml_diff>

<commit_message>
Updated skills TODO.xlsx file.
</commit_message>
<xml_diff>
--- a/trunk/dist/game/data/stats/skills/TODO.xlsx
+++ b/trunk/dist/game/data/stats/skills/TODO.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1200" uniqueCount="638">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1217" uniqueCount="637">
   <si>
     <t>Skill Name</t>
   </si>
@@ -1827,9 +1827,6 @@
   </si>
   <si>
     <t>Aqua Crash - Speed Decrease</t>
-  </si>
-  <si>
-    <t>No</t>
   </si>
   <si>
     <t>Aqua Crash - Freeze</t>
@@ -2364,7 +2361,7 @@
   <dimension ref="A1:G679"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="C618" sqref="C618"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -2411,7 +2408,7 @@
       </c>
       <c r="G2" s="2">
         <f>COUNTIF(C2:C679,"yes")</f>
-        <v>511</v>
+        <v>529</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -2430,7 +2427,7 @@
       </c>
       <c r="G3">
         <f>678-G2</f>
-        <v>167</v>
+        <v>149</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -2449,7 +2446,7 @@
       </c>
       <c r="G4" s="4">
         <f>100-(G3*100)/678</f>
-        <v>75.368731563421832</v>
+        <v>78.023598820058993</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -3859,7 +3856,9 @@
       <c r="B122" s="7">
         <v>10106</v>
       </c>
-      <c r="C122" s="14"/>
+      <c r="C122" s="8" t="s">
+        <v>548</v>
+      </c>
       <c r="D122" s="12"/>
     </row>
     <row r="123" spans="1:4">
@@ -4222,7 +4221,7 @@
     </row>
     <row r="153" spans="1:4">
       <c r="A153" s="6" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="B153" s="7">
         <v>10289</v>
@@ -4585,7 +4584,9 @@
       <c r="B183" s="7">
         <v>10333</v>
       </c>
-      <c r="C183" s="14"/>
+      <c r="C183" s="14" t="s">
+        <v>548</v>
+      </c>
       <c r="D183" s="12"/>
     </row>
     <row r="184" spans="1:4">
@@ -4605,7 +4606,9 @@
       <c r="B185" s="7">
         <v>10335</v>
       </c>
-      <c r="C185" s="14"/>
+      <c r="C185" s="14" t="s">
+        <v>548</v>
+      </c>
       <c r="D185" s="12"/>
     </row>
     <row r="186" spans="1:4">
@@ -5241,7 +5244,9 @@
       <c r="B239" s="7">
         <v>10705</v>
       </c>
-      <c r="C239" s="14"/>
+      <c r="C239" s="8" t="s">
+        <v>548</v>
+      </c>
       <c r="D239" s="12"/>
     </row>
     <row r="240" spans="1:4">
@@ -5799,7 +5804,9 @@
       <c r="B287" s="7">
         <v>10952</v>
       </c>
-      <c r="C287" s="14"/>
+      <c r="C287" s="8" t="s">
+        <v>548</v>
+      </c>
       <c r="D287" s="13"/>
     </row>
     <row r="288" spans="1:4">
@@ -5809,7 +5816,9 @@
       <c r="B288" s="7">
         <v>10953</v>
       </c>
-      <c r="C288" s="14"/>
+      <c r="C288" s="8" t="s">
+        <v>548</v>
+      </c>
       <c r="D288" s="13"/>
     </row>
     <row r="289" spans="1:4">
@@ -5819,7 +5828,9 @@
       <c r="B289" s="7">
         <v>10954</v>
       </c>
-      <c r="C289" s="14"/>
+      <c r="C289" s="8" t="s">
+        <v>548</v>
+      </c>
       <c r="D289" s="13"/>
     </row>
     <row r="290" spans="1:4">
@@ -5829,7 +5840,9 @@
       <c r="B290" s="7">
         <v>10955</v>
       </c>
-      <c r="C290" s="14"/>
+      <c r="C290" s="8" t="s">
+        <v>548</v>
+      </c>
       <c r="D290" s="13"/>
     </row>
     <row r="291" spans="1:4">
@@ -6565,9 +6578,7 @@
       <c r="B358" s="7">
         <v>11178</v>
       </c>
-      <c r="C358" s="8" t="s">
-        <v>604</v>
-      </c>
+      <c r="C358" s="8"/>
       <c r="D358" s="12"/>
     </row>
     <row r="359" spans="1:4">
@@ -6613,7 +6624,9 @@
       <c r="B362" s="7">
         <v>11186</v>
       </c>
-      <c r="C362" s="14"/>
+      <c r="C362" s="8" t="s">
+        <v>548</v>
+      </c>
       <c r="D362" s="12"/>
     </row>
     <row r="363" spans="1:4">
@@ -6623,7 +6636,9 @@
       <c r="B363" s="7">
         <v>11187</v>
       </c>
-      <c r="C363" s="14"/>
+      <c r="C363" s="8" t="s">
+        <v>548</v>
+      </c>
       <c r="D363" s="12"/>
     </row>
     <row r="364" spans="1:4">
@@ -6678,7 +6693,7 @@
     </row>
     <row r="369" spans="1:4">
       <c r="A369" s="6" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="B369" s="7">
         <v>11195</v>
@@ -7452,7 +7467,7 @@
     </row>
     <row r="438" spans="1:4">
       <c r="A438" s="6" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="B438" s="7">
         <v>11369</v>
@@ -7462,7 +7477,7 @@
     </row>
     <row r="439" spans="1:4">
       <c r="A439" s="6" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="B439" s="7">
         <v>11370</v>
@@ -7472,7 +7487,7 @@
     </row>
     <row r="440" spans="1:4">
       <c r="A440" s="6" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="B440" s="7">
         <v>11371</v>
@@ -7482,7 +7497,7 @@
     </row>
     <row r="441" spans="1:4">
       <c r="A441" s="6" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="B441" s="7">
         <v>11372</v>
@@ -7492,7 +7507,7 @@
     </row>
     <row r="442" spans="1:4">
       <c r="A442" s="6" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="B442" s="7">
         <v>11373</v>
@@ -7502,7 +7517,7 @@
     </row>
     <row r="443" spans="1:4">
       <c r="A443" s="6" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="B443" s="7">
         <v>11374</v>
@@ -7512,7 +7527,7 @@
     </row>
     <row r="444" spans="1:4">
       <c r="A444" s="6" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="B444" s="7">
         <v>11389</v>
@@ -7522,7 +7537,7 @@
     </row>
     <row r="445" spans="1:4">
       <c r="A445" s="6" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="B445" s="7">
         <v>11391</v>
@@ -7873,7 +7888,9 @@
       <c r="B474" s="7">
         <v>11536</v>
       </c>
-      <c r="C474" s="14"/>
+      <c r="C474" s="8" t="s">
+        <v>548</v>
+      </c>
       <c r="D474" s="12"/>
     </row>
     <row r="475" spans="1:4">
@@ -9334,7 +9351,7 @@
     </row>
     <row r="599" spans="1:4">
       <c r="A599" s="6" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="B599" s="7">
         <v>17920</v>
@@ -9344,7 +9361,7 @@
     </row>
     <row r="600" spans="1:4">
       <c r="A600" s="6" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="B600" s="7">
         <v>17943</v>
@@ -9376,7 +9393,7 @@
     </row>
     <row r="603" spans="1:4">
       <c r="A603" s="6" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="B603" s="7">
         <v>19203</v>
@@ -9386,7 +9403,7 @@
     </row>
     <row r="604" spans="1:4">
       <c r="A604" s="6" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="B604" s="7">
         <v>19204</v>
@@ -9396,7 +9413,7 @@
     </row>
     <row r="605" spans="1:4">
       <c r="A605" s="6" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="B605" s="7">
         <v>19205</v>
@@ -9406,7 +9423,7 @@
     </row>
     <row r="606" spans="1:4">
       <c r="A606" s="6" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="B606" s="7">
         <v>19206</v>
@@ -9416,7 +9433,7 @@
     </row>
     <row r="607" spans="1:4">
       <c r="A607" s="6" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="B607" s="7">
         <v>19207</v>
@@ -9426,7 +9443,7 @@
     </row>
     <row r="608" spans="1:4">
       <c r="A608" s="6" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="B608" s="7">
         <v>19208</v>
@@ -9436,7 +9453,7 @@
     </row>
     <row r="609" spans="1:4">
       <c r="A609" s="6" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="B609" s="7">
         <v>19209</v>
@@ -9446,7 +9463,7 @@
     </row>
     <row r="610" spans="1:4">
       <c r="A610" s="6" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="B610" s="7">
         <v>19210</v>
@@ -9456,7 +9473,7 @@
     </row>
     <row r="611" spans="1:4">
       <c r="A611" s="6" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="B611" s="7">
         <v>19212</v>
@@ -9466,67 +9483,79 @@
     </row>
     <row r="612" spans="1:4">
       <c r="A612" s="6" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="B612" s="7">
         <v>19213</v>
       </c>
-      <c r="C612" s="14"/>
+      <c r="C612" s="14" t="s">
+        <v>548</v>
+      </c>
       <c r="D612" s="12"/>
     </row>
     <row r="613" spans="1:4">
       <c r="A613" s="6" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="B613" s="7">
         <v>19214</v>
       </c>
-      <c r="C613" s="14"/>
+      <c r="C613" s="14" t="s">
+        <v>548</v>
+      </c>
       <c r="D613" s="12"/>
     </row>
     <row r="614" spans="1:4">
       <c r="A614" s="6" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="B614" s="7">
         <v>19215</v>
       </c>
-      <c r="C614" s="14"/>
+      <c r="C614" s="14" t="s">
+        <v>548</v>
+      </c>
       <c r="D614" s="12"/>
     </row>
     <row r="615" spans="1:4">
       <c r="A615" s="6" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="B615" s="7">
         <v>19216</v>
       </c>
-      <c r="C615" s="14"/>
+      <c r="C615" s="14" t="s">
+        <v>548</v>
+      </c>
       <c r="D615" s="13"/>
     </row>
     <row r="616" spans="1:4">
       <c r="A616" s="6" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="B616" s="7">
         <v>19217</v>
       </c>
-      <c r="C616" s="14"/>
+      <c r="C616" s="14" t="s">
+        <v>548</v>
+      </c>
       <c r="D616" s="13"/>
     </row>
     <row r="617" spans="1:4">
       <c r="A617" s="6" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="B617" s="7">
         <v>19218</v>
       </c>
-      <c r="C617" s="14"/>
+      <c r="C617" s="14" t="s">
+        <v>548</v>
+      </c>
       <c r="D617" s="13"/>
     </row>
     <row r="618" spans="1:4">
       <c r="A618" s="6" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="B618" s="7">
         <v>19220</v>
@@ -9536,12 +9565,14 @@
     </row>
     <row r="619" spans="1:4">
       <c r="A619" s="6" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="B619" s="7">
         <v>19228</v>
       </c>
-      <c r="C619" s="14"/>
+      <c r="C619" s="8" t="s">
+        <v>548</v>
+      </c>
       <c r="D619" s="13"/>
     </row>
     <row r="620" spans="1:4">
@@ -9960,7 +9991,7 @@
     </row>
     <row r="656" spans="1:4">
       <c r="A656" s="6" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="B656" s="7">
         <v>30510</v>
@@ -10164,7 +10195,7 @@
     </row>
     <row r="675" spans="1:4">
       <c r="A675" s="6" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="B675" s="7">
         <v>30546</v>
@@ -10176,7 +10207,7 @@
     </row>
     <row r="676" spans="1:4">
       <c r="A676" s="6" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="B676" s="7">
         <v>30547</v>
@@ -10200,7 +10231,7 @@
     </row>
     <row r="678" spans="1:4">
       <c r="A678" s="6" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="B678" s="7">
         <v>30604</v>
@@ -10233,9 +10264,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B372"/>
   <sheetViews>
-    <sheetView topLeftCell="A148" workbookViewId="0">
-      <selection activeCell="A169" sqref="A169"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>

</xml_diff>

<commit_message>
New Auras and some skill fixes. Contributed by hitnar.
</commit_message>
<xml_diff>
--- a/trunk/dist/game/data/stats/skills/TODO.xlsx
+++ b/trunk/dist/game/data/stats/skills/TODO.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1217" uniqueCount="637">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1221" uniqueCount="637">
   <si>
     <t>Skill Name</t>
   </si>
@@ -2360,8 +2360,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G679"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C618" sqref="C618"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -2408,7 +2408,7 @@
       </c>
       <c r="G2" s="2">
         <f>COUNTIF(C2:C679,"yes")</f>
-        <v>529</v>
+        <v>533</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -2427,7 +2427,7 @@
       </c>
       <c r="G3">
         <f>678-G2</f>
-        <v>149</v>
+        <v>145</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -2446,7 +2446,7 @@
       </c>
       <c r="G4" s="4">
         <f>100-(G3*100)/678</f>
-        <v>78.023598820058993</v>
+        <v>78.61356932153393</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -3836,7 +3836,9 @@
       <c r="B120" s="7">
         <v>10104</v>
       </c>
-      <c r="C120" s="14"/>
+      <c r="C120" s="8" t="s">
+        <v>548</v>
+      </c>
       <c r="D120" s="12"/>
     </row>
     <row r="121" spans="1:4">
@@ -3846,7 +3848,9 @@
       <c r="B121" s="7">
         <v>10105</v>
       </c>
-      <c r="C121" s="14"/>
+      <c r="C121" s="8" t="s">
+        <v>548</v>
+      </c>
       <c r="D121" s="12"/>
     </row>
     <row r="122" spans="1:4">
@@ -3868,7 +3872,9 @@
       <c r="B123" s="7">
         <v>10107</v>
       </c>
-      <c r="C123" s="14"/>
+      <c r="C123" s="8" t="s">
+        <v>548</v>
+      </c>
       <c r="D123" s="12"/>
     </row>
     <row r="124" spans="1:4">
@@ -4574,7 +4580,9 @@
       <c r="B182" s="7">
         <v>10332</v>
       </c>
-      <c r="C182" s="14"/>
+      <c r="C182" s="8" t="s">
+        <v>548</v>
+      </c>
       <c r="D182" s="12"/>
     </row>
     <row r="183" spans="1:4">

</xml_diff>

<commit_message>
Armor Breaker and Power Bluff skills. Contributed by hitnar.
</commit_message>
<xml_diff>
--- a/trunk/dist/game/data/stats/skills/TODO.xlsx
+++ b/trunk/dist/game/data/stats/skills/TODO.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1221" uniqueCount="637">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1222" uniqueCount="637">
   <si>
     <t>Skill Name</t>
   </si>
@@ -2360,7 +2360,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G679"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
@@ -2408,7 +2408,7 @@
       </c>
       <c r="G2" s="2">
         <f>COUNTIF(C2:C679,"yes")</f>
-        <v>533</v>
+        <v>534</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -2427,7 +2427,7 @@
       </c>
       <c r="G3">
         <f>678-G2</f>
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -2446,7 +2446,7 @@
       </c>
       <c r="G4" s="4">
         <f>100-(G3*100)/678</f>
-        <v>78.61356932153393</v>
+        <v>78.761061946902657</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -5232,7 +5232,9 @@
       <c r="B237" s="7">
         <v>10703</v>
       </c>
-      <c r="C237" s="14"/>
+      <c r="C237" s="8" t="s">
+        <v>548</v>
+      </c>
       <c r="D237" s="13"/>
     </row>
     <row r="238" spans="1:4">

</xml_diff>

<commit_message>
A couple of skills work. Contributed by hitnar.
</commit_message>
<xml_diff>
--- a/trunk/dist/game/data/stats/skills/TODO.xlsx
+++ b/trunk/dist/game/data/stats/skills/TODO.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1222" uniqueCount="637">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1225" uniqueCount="637">
   <si>
     <t>Skill Name</t>
   </si>
@@ -2408,7 +2408,7 @@
       </c>
       <c r="G2" s="2">
         <f>COUNTIF(C2:C679,"yes")</f>
-        <v>534</v>
+        <v>537</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -2427,7 +2427,7 @@
       </c>
       <c r="G3">
         <f>678-G2</f>
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -2446,7 +2446,7 @@
       </c>
       <c r="G4" s="4">
         <f>100-(G3*100)/678</f>
-        <v>78.761061946902657</v>
+        <v>79.203539823008853</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -7036,7 +7036,9 @@
       <c r="B399" s="7">
         <v>11273</v>
       </c>
-      <c r="C399" s="14"/>
+      <c r="C399" s="8" t="s">
+        <v>548</v>
+      </c>
       <c r="D399" s="13"/>
     </row>
     <row r="400" spans="1:4">
@@ -7056,7 +7058,9 @@
       <c r="B401" s="7">
         <v>11276</v>
       </c>
-      <c r="C401" s="14"/>
+      <c r="C401" s="8" t="s">
+        <v>548</v>
+      </c>
       <c r="D401" s="13"/>
     </row>
     <row r="402" spans="1:4">
@@ -7102,7 +7106,9 @@
       <c r="B405" s="7">
         <v>11296</v>
       </c>
-      <c r="C405" s="14"/>
+      <c r="C405" s="8" t="s">
+        <v>548</v>
+      </c>
       <c r="D405" s="13"/>
     </row>
     <row r="406" spans="1:4">

</xml_diff>

<commit_message>
Mark of Retriever handler. Contributed by hitnar.
</commit_message>
<xml_diff>
--- a/trunk/dist/game/data/stats/skills/TODO.xlsx
+++ b/trunk/dist/game/data/stats/skills/TODO.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1225" uniqueCount="637">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1229" uniqueCount="637">
   <si>
     <t>Skill Name</t>
   </si>
@@ -2408,7 +2408,7 @@
       </c>
       <c r="G2" s="2">
         <f>COUNTIF(C2:C679,"yes")</f>
-        <v>537</v>
+        <v>541</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -2427,7 +2427,7 @@
       </c>
       <c r="G3">
         <f>678-G2</f>
-        <v>141</v>
+        <v>137</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -2446,7 +2446,7 @@
       </c>
       <c r="G4" s="4">
         <f>100-(G3*100)/678</f>
-        <v>79.203539823008853</v>
+        <v>79.793510324483776</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -6886,7 +6886,9 @@
       <c r="B385" s="7">
         <v>11259</v>
       </c>
-      <c r="C385" s="14"/>
+      <c r="C385" s="8" t="s">
+        <v>548</v>
+      </c>
       <c r="D385" s="12"/>
     </row>
     <row r="386" spans="1:4">
@@ -6896,7 +6898,9 @@
       <c r="B386" s="7">
         <v>11260</v>
       </c>
-      <c r="C386" s="14"/>
+      <c r="C386" s="8" t="s">
+        <v>548</v>
+      </c>
       <c r="D386" s="13"/>
     </row>
     <row r="387" spans="1:4">
@@ -6906,7 +6910,9 @@
       <c r="B387" s="7">
         <v>11261</v>
       </c>
-      <c r="C387" s="14"/>
+      <c r="C387" s="8" t="s">
+        <v>548</v>
+      </c>
       <c r="D387" s="13"/>
     </row>
     <row r="388" spans="1:4">
@@ -6916,7 +6922,9 @@
       <c r="B388" s="7">
         <v>11262</v>
       </c>
-      <c r="C388" s="14"/>
+      <c r="C388" s="8" t="s">
+        <v>548</v>
+      </c>
       <c r="D388" s="13"/>
     </row>
     <row r="389" spans="1:4">

</xml_diff>

<commit_message>
Some skill fixes. Contributed by Mathael.
</commit_message>
<xml_diff>
--- a/trunk/dist/game/data/stats/skills/TODO.xlsx
+++ b/trunk/dist/game/data/stats/skills/TODO.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1229" uniqueCount="637">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1232" uniqueCount="637">
   <si>
     <t>Skill Name</t>
   </si>
@@ -2408,7 +2408,7 @@
       </c>
       <c r="G2" s="2">
         <f>COUNTIF(C2:C679,"yes")</f>
-        <v>541</v>
+        <v>544</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -2427,7 +2427,7 @@
       </c>
       <c r="G3">
         <f>678-G2</f>
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -2446,7 +2446,7 @@
       </c>
       <c r="G4" s="4">
         <f>100-(G3*100)/678</f>
-        <v>79.793510324483776</v>
+        <v>80.235988200589972</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -6934,7 +6934,9 @@
       <c r="B389" s="7">
         <v>11263</v>
       </c>
-      <c r="C389" s="14"/>
+      <c r="C389" s="8" t="s">
+        <v>548</v>
+      </c>
       <c r="D389" s="13"/>
     </row>
     <row r="390" spans="1:4">
@@ -7446,7 +7448,9 @@
       <c r="B433" s="7">
         <v>11356</v>
       </c>
-      <c r="C433" s="14"/>
+      <c r="C433" s="14" t="s">
+        <v>548</v>
+      </c>
       <c r="D433" s="13"/>
     </row>
     <row r="434" spans="1:4">
@@ -7486,7 +7490,9 @@
       <c r="B437" s="7">
         <v>11365</v>
       </c>
-      <c r="C437" s="14"/>
+      <c r="C437" s="14" t="s">
+        <v>548</v>
+      </c>
       <c r="D437" s="13"/>
     </row>
     <row r="438" spans="1:4">

</xml_diff>

<commit_message>
Skill improvements. Contributed by hitnar.
</commit_message>
<xml_diff>
--- a/trunk/dist/game/data/stats/skills/TODO.xlsx
+++ b/trunk/dist/game/data/stats/skills/TODO.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1232" uniqueCount="637">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1240" uniqueCount="637">
   <si>
     <t>Skill Name</t>
   </si>
@@ -2408,7 +2408,7 @@
       </c>
       <c r="G2" s="2">
         <f>COUNTIF(C2:C679,"yes")</f>
-        <v>544</v>
+        <v>552</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -2427,7 +2427,7 @@
       </c>
       <c r="G3">
         <f>678-G2</f>
-        <v>134</v>
+        <v>126</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -2446,7 +2446,7 @@
       </c>
       <c r="G4" s="4">
         <f>100-(G3*100)/678</f>
-        <v>80.235988200589972</v>
+        <v>81.415929203539818</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -6070,7 +6070,7 @@
         <v>271</v>
       </c>
       <c r="B309" s="7">
-        <v>11040</v>
+        <v>11047</v>
       </c>
       <c r="C309" s="8" t="s">
         <v>548</v>
@@ -6120,7 +6120,9 @@
       <c r="B313" s="7">
         <v>11049</v>
       </c>
-      <c r="C313" s="14"/>
+      <c r="C313" s="8" t="s">
+        <v>548</v>
+      </c>
       <c r="D313" s="13"/>
     </row>
     <row r="314" spans="1:4">
@@ -6130,7 +6132,9 @@
       <c r="B314" s="7">
         <v>11050</v>
       </c>
-      <c r="C314" s="14"/>
+      <c r="C314" s="8" t="s">
+        <v>548</v>
+      </c>
       <c r="D314" s="13"/>
     </row>
     <row r="315" spans="1:4">
@@ -6140,7 +6144,9 @@
       <c r="B315" s="7">
         <v>11052</v>
       </c>
-      <c r="C315" s="14"/>
+      <c r="C315" s="8" t="s">
+        <v>548</v>
+      </c>
       <c r="D315" s="13"/>
     </row>
     <row r="316" spans="1:4">
@@ -6162,7 +6168,9 @@
       <c r="B317" s="7">
         <v>11056</v>
       </c>
-      <c r="C317" s="14"/>
+      <c r="C317" s="8" t="s">
+        <v>548</v>
+      </c>
       <c r="D317" s="12"/>
     </row>
     <row r="318" spans="1:4">
@@ -6172,7 +6180,9 @@
       <c r="B318" s="7">
         <v>11057</v>
       </c>
-      <c r="C318" s="14"/>
+      <c r="C318" s="8" t="s">
+        <v>548</v>
+      </c>
       <c r="D318" s="12"/>
     </row>
     <row r="319" spans="1:4">
@@ -6204,7 +6214,9 @@
       <c r="B321" s="7">
         <v>11064</v>
       </c>
-      <c r="C321" s="14"/>
+      <c r="C321" s="8" t="s">
+        <v>548</v>
+      </c>
       <c r="D321" s="12"/>
     </row>
     <row r="322" spans="1:4">
@@ -6250,7 +6262,9 @@
       <c r="B325" s="7">
         <v>11068</v>
       </c>
-      <c r="C325" s="14"/>
+      <c r="C325" s="8" t="s">
+        <v>548</v>
+      </c>
       <c r="D325" s="12"/>
     </row>
     <row r="326" spans="1:4">
@@ -6372,7 +6386,9 @@
       <c r="B337" s="7">
         <v>11094</v>
       </c>
-      <c r="C337" s="14"/>
+      <c r="C337" s="8" t="s">
+        <v>548</v>
+      </c>
       <c r="D337" s="12"/>
     </row>
     <row r="338" spans="1:4">

</xml_diff>